<commit_message>
Refine Quote Enhancement v1
</commit_message>
<xml_diff>
--- a/src/pricing/simpleFiles/MBC/Dom-ST.xlsx
+++ b/src/pricing/simpleFiles/MBC/Dom-ST.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="24" documentId="11_8436E50C0BB0DF5FCFBA572784B390D0AEE9516F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B99BD56-9FEB-4FAA-8311-4A0A64F33F1D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13650" firstSheet="25" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29010" windowHeight="13650" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan_Info" sheetId="2" r:id="rId1"/>
@@ -11973,7 +11973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -54425,7 +54425,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>